<commit_message>
Fixed timer not being saved to EEPROM position 0 Re-enabled UDP mode, worked ALL night so seems stable Enabled auto restart by MQTT... saves to EEPROM, and loads... good for testing...
</commit_message>
<xml_diff>
--- a/ESP memory Map.xlsx
+++ b/ESP memory Map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="33">
   <si>
     <t>Device Name</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>var10</t>
+  </si>
+  <si>
+    <t>AutoRestart</t>
   </si>
 </sst>
 </file>
@@ -276,33 +279,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
@@ -310,6 +295,25 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -652,7 +656,7 @@
   <dimension ref="A2:AH18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+      <selection activeCell="C8" sqref="C8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -800,40 +804,40 @@
       <c r="A4">
         <v>32</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
       <c r="AH4">
         <v>63</v>
       </c>
@@ -842,40 +846,40 @@
       <c r="A5">
         <v>64</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
       <c r="AH5">
         <v>95</v>
       </c>
@@ -884,40 +888,40 @@
       <c r="A6">
         <v>96</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
       <c r="AH6">
         <v>127</v>
       </c>
@@ -926,24 +930,27 @@
       <c r="A7">
         <v>128</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="20"/>
+      <c r="J7" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="AH7">
         <v>159</v>
@@ -953,60 +960,60 @@
       <c r="A8">
         <v>160</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="7">
         <v>0</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q8" s="16" t="s">
+      <c r="Q8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T8" s="19" t="s">
+      <c r="R8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U8" s="20" t="s">
+      <c r="U8" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH8">
@@ -1017,60 +1024,60 @@
       <c r="A9">
         <v>192</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="N9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="Q9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" s="19" t="s">
+      <c r="R9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U9" s="20" t="s">
+      <c r="U9" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH9">
@@ -1081,60 +1088,60 @@
       <c r="A10">
         <v>224</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="7">
         <v>2</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="18" t="s">
+      <c r="P10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="16" t="s">
+      <c r="Q10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T10" s="19" t="s">
+      <c r="R10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U10" s="20" t="s">
+      <c r="U10" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH10">
@@ -1145,60 +1152,60 @@
       <c r="A11">
         <v>256</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="P11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11" s="19" t="s">
+      <c r="R11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U11" s="20" t="s">
+      <c r="U11" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH11">
@@ -1209,60 +1216,60 @@
       <c r="A12">
         <v>288</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="7">
         <v>4</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="18" t="s">
+      <c r="P12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q12" s="16" t="s">
+      <c r="Q12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="19" t="s">
+      <c r="R12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U12" s="20" t="s">
+      <c r="U12" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH12">
@@ -1273,60 +1280,60 @@
       <c r="A13">
         <v>320</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="7">
         <v>5</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="17" t="s">
+      <c r="N13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="18" t="s">
+      <c r="P13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q13" s="16" t="s">
+      <c r="Q13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T13" s="19" t="s">
+      <c r="R13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U13" s="20" t="s">
+      <c r="U13" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH13">
@@ -1337,60 +1344,60 @@
       <c r="A14">
         <v>352</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="7">
         <v>6</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="16"/>
+      <c r="G14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q14" s="16" t="s">
+      <c r="Q14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T14" s="19" t="s">
+      <c r="R14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U14" s="20" t="s">
+      <c r="U14" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH14">
@@ -1401,60 +1408,60 @@
       <c r="A15">
         <v>384</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="7">
         <v>7</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="17" t="s">
+      <c r="N15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="18" t="s">
+      <c r="P15" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="16" t="s">
+      <c r="Q15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="19" t="s">
+      <c r="R15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U15" s="20" t="s">
+      <c r="U15" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH15">
@@ -1465,60 +1472,60 @@
       <c r="A16">
         <v>416</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="7">
         <v>8</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N16" s="17" t="s">
+      <c r="N16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q16" s="16" t="s">
+      <c r="Q16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T16" s="19" t="s">
+      <c r="R16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U16" s="20" t="s">
+      <c r="U16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH16">
@@ -1529,60 +1536,60 @@
       <c r="A17">
         <v>448</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="7">
         <v>9</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13" t="s">
+      <c r="D17" s="15"/>
+      <c r="E17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="7" t="s">
+      <c r="F17" s="16"/>
+      <c r="G17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O17" s="15" t="s">
+      <c r="O17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q17" s="16" t="s">
+      <c r="Q17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T17" s="19" t="s">
+      <c r="R17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U17" s="20" t="s">
+      <c r="U17" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH17">
@@ -1593,60 +1600,60 @@
       <c r="A18">
         <v>480</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="7">
         <v>10</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P18" s="18" t="s">
+      <c r="P18" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="Q18" s="16" t="s">
+      <c r="Q18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T18" s="19" t="s">
+      <c r="R18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="U18" s="20" t="s">
+      <c r="U18" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AH18">
@@ -1655,6 +1662,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B4:AG4"/>
+    <mergeCell ref="B5:AG5"/>
+    <mergeCell ref="B6:AG6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="C15:D15"/>
@@ -1663,24 +1688,6 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B4:AG4"/>
-    <mergeCell ref="B5:AG5"/>
-    <mergeCell ref="B6:AG6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>